<commit_message>
updates on stoichi vs CEF
</commit_message>
<xml_diff>
--- a/tc_df_FullEquil_check_filter.xlsx
+++ b/tc_df_FullEquil_check_filter.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G151"/>
+  <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,17 +446,17 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>np(HEMATITE)</t>
+          <t>np(CORUNDUM)</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>np(MAGNETITE)</t>
+          <t>np(SPINEL)</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>np(WUSTITE)</t>
+          <t>np(HALITE)</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -464,11 +464,6 @@
           <t>np(BCC_A2)</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>np(LIQUID)</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -489,9 +484,6 @@
       <c r="F2" t="n">
         <v>1.00000000002635</v>
       </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -510,10 +502,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>1.000000000025243</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
+        <v>1.000000000025242</v>
       </c>
     </row>
     <row r="4">
@@ -533,10 +522,7 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>1.000000000024136</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
+        <v>1.000000000024135</v>
       </c>
     </row>
     <row r="5">
@@ -556,10 +542,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>1.000000000023028</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
+        <v>1.000000000023027</v>
       </c>
     </row>
     <row r="6">
@@ -579,10 +562,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>1.000000000021921</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
+        <v>1.00000000002192</v>
       </c>
     </row>
     <row r="7">
@@ -604,9 +584,6 @@
       <c r="F7" t="n">
         <v>1.000000000020813</v>
       </c>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -625,10 +602,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>1.000000000019706</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0</v>
+        <v>1.000000000019705</v>
       </c>
     </row>
     <row r="9">
@@ -648,10 +622,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>1.000000000018599</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0</v>
+        <v>1.000000000018598</v>
       </c>
     </row>
     <row r="10">
@@ -671,10 +642,7 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>1.000000000017491</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0</v>
+        <v>1.00000000001749</v>
       </c>
     </row>
     <row r="11">
@@ -694,10 +662,7 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>1.000000000016384</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0</v>
+        <v>1.000000000016383</v>
       </c>
     </row>
     <row r="12">
@@ -719,9 +684,6 @@
       <c r="F12" t="n">
         <v>1.000000000015276</v>
       </c>
-      <c r="G12" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -740,10 +702,7 @@
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>1.000000000014169</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0</v>
+        <v>1.000000000014168</v>
       </c>
     </row>
     <row r="14">
@@ -763,10 +722,7 @@
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>1.000000000013062</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0</v>
+        <v>1.000000000013061</v>
       </c>
     </row>
     <row r="15">
@@ -788,9 +744,6 @@
       <c r="F15" t="n">
         <v>1.000000000011954</v>
       </c>
-      <c r="G15" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -809,10 +762,7 @@
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>1.000000000010847</v>
-      </c>
-      <c r="G16" t="n">
-        <v>0</v>
+        <v>1.000000000010846</v>
       </c>
     </row>
     <row r="17">
@@ -832,10 +782,7 @@
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>1.00000000000974</v>
-      </c>
-      <c r="G17" t="n">
-        <v>0</v>
+        <v>1.000000000009739</v>
       </c>
     </row>
     <row r="18">
@@ -855,10 +802,7 @@
         <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>1.000000000008632</v>
-      </c>
-      <c r="G18" t="n">
-        <v>0</v>
+        <v>1.000000000008631</v>
       </c>
     </row>
     <row r="19">
@@ -878,10 +822,7 @@
         <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>1.000000000007525</v>
-      </c>
-      <c r="G19" t="n">
-        <v>0</v>
+        <v>1.000000000007524</v>
       </c>
     </row>
     <row r="20">
@@ -901,10 +842,7 @@
         <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>1.000000000006418</v>
-      </c>
-      <c r="G20" t="n">
-        <v>0</v>
+        <v>1.000000000006417</v>
       </c>
     </row>
     <row r="21">
@@ -924,10 +862,7 @@
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>1.00000000000531</v>
-      </c>
-      <c r="G21" t="n">
-        <v>0</v>
+        <v>1.000000000005309</v>
       </c>
     </row>
     <row r="22">
@@ -947,10 +882,7 @@
         <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>1.000000000004203</v>
-      </c>
-      <c r="G22" t="n">
-        <v>0</v>
+        <v>1.000000000004202</v>
       </c>
     </row>
     <row r="23">
@@ -970,10 +902,7 @@
         <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>1.000000000003095</v>
-      </c>
-      <c r="G23" t="n">
-        <v>0</v>
+        <v>1.000000000003094</v>
       </c>
     </row>
     <row r="24">
@@ -993,10 +922,7 @@
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>1.000000000001988</v>
-      </c>
-      <c r="G24" t="n">
-        <v>0</v>
+        <v>1.000000000001987</v>
       </c>
     </row>
     <row r="25">
@@ -1018,9 +944,6 @@
       <c r="F25" t="n">
         <v>1.00000000000088</v>
       </c>
-      <c r="G25" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1041,9 +964,6 @@
       <c r="F26" t="n">
         <v>1</v>
       </c>
-      <c r="G26" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1064,9 +984,6 @@
       <c r="F27" t="n">
         <v>1</v>
       </c>
-      <c r="G27" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1087,9 +1004,6 @@
       <c r="F28" t="n">
         <v>1</v>
       </c>
-      <c r="G28" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1110,9 +1024,6 @@
       <c r="F29" t="n">
         <v>1</v>
       </c>
-      <c r="G29" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -1133,9 +1044,6 @@
       <c r="F30" t="n">
         <v>1</v>
       </c>
-      <c r="G30" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -1156,9 +1064,6 @@
       <c r="F31" t="n">
         <v>1</v>
       </c>
-      <c r="G31" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -1179,9 +1084,6 @@
       <c r="F32" t="n">
         <v>1</v>
       </c>
-      <c r="G32" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -1202,9 +1104,6 @@
       <c r="F33" t="n">
         <v>1</v>
       </c>
-      <c r="G33" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -1225,9 +1124,6 @@
       <c r="F34" t="n">
         <v>1</v>
       </c>
-      <c r="G34" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -1248,9 +1144,6 @@
       <c r="F35" t="n">
         <v>1</v>
       </c>
-      <c r="G35" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -1271,9 +1164,6 @@
       <c r="F36" t="n">
         <v>1</v>
       </c>
-      <c r="G36" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -1286,15 +1176,12 @@
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>1</v>
+        <v>0.9999999999981205</v>
       </c>
       <c r="E37" t="n">
         <v>0</v>
       </c>
       <c r="F37" t="n">
-        <v>0</v>
-      </c>
-      <c r="G37" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1309,15 +1196,12 @@
         <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>1</v>
+        <v>0.9999999999982608</v>
       </c>
       <c r="E38" t="n">
         <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>0</v>
-      </c>
-      <c r="G38" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1332,15 +1216,12 @@
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>1</v>
+        <v>0.9999999999984015</v>
       </c>
       <c r="E39" t="n">
         <v>0</v>
       </c>
       <c r="F39" t="n">
-        <v>0</v>
-      </c>
-      <c r="G39" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1355,15 +1236,12 @@
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>1</v>
+        <v>0.9999999999985418</v>
       </c>
       <c r="E40" t="n">
         <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>0</v>
-      </c>
-      <c r="G40" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1378,15 +1256,12 @@
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>1</v>
+        <v>0.9999999999986831</v>
       </c>
       <c r="E41" t="n">
         <v>0</v>
       </c>
       <c r="F41" t="n">
-        <v>0</v>
-      </c>
-      <c r="G41" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1401,15 +1276,12 @@
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>1</v>
+        <v>0.9999999999988229</v>
       </c>
       <c r="E42" t="n">
         <v>0</v>
       </c>
       <c r="F42" t="n">
-        <v>0</v>
-      </c>
-      <c r="G42" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1424,15 +1296,12 @@
         <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>1</v>
+        <v>0.9999999999989638</v>
       </c>
       <c r="E43" t="n">
         <v>0</v>
       </c>
       <c r="F43" t="n">
-        <v>0</v>
-      </c>
-      <c r="G43" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1447,15 +1316,12 @@
         <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>1</v>
+        <v>0.9999999999991048</v>
       </c>
       <c r="E44" t="n">
         <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>0</v>
-      </c>
-      <c r="G44" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1470,15 +1336,12 @@
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>1</v>
+        <v>0.9999999999992452</v>
       </c>
       <c r="E45" t="n">
         <v>0</v>
       </c>
       <c r="F45" t="n">
-        <v>0</v>
-      </c>
-      <c r="G45" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1493,15 +1356,12 @@
         <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>1</v>
+        <v>0.9999999999993862</v>
       </c>
       <c r="E46" t="n">
         <v>0</v>
       </c>
       <c r="F46" t="n">
-        <v>0</v>
-      </c>
-      <c r="G46" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1516,15 +1376,12 @@
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>1</v>
+        <v>0.9999999999995266</v>
       </c>
       <c r="E47" t="n">
         <v>0</v>
       </c>
       <c r="F47" t="n">
-        <v>0</v>
-      </c>
-      <c r="G47" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1539,15 +1396,12 @@
         <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>1</v>
+        <v>0.9999999999996673</v>
       </c>
       <c r="E48" t="n">
         <v>0</v>
       </c>
       <c r="F48" t="n">
-        <v>0</v>
-      </c>
-      <c r="G48" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1562,15 +1416,12 @@
         <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>1</v>
+        <v>0.9999999999998078</v>
       </c>
       <c r="E49" t="n">
         <v>0</v>
       </c>
       <c r="F49" t="n">
-        <v>0</v>
-      </c>
-      <c r="G49" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1585,15 +1436,12 @@
         <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>1</v>
+        <v>0.9999999999999488</v>
       </c>
       <c r="E50" t="n">
         <v>0</v>
       </c>
       <c r="F50" t="n">
-        <v>0</v>
-      </c>
-      <c r="G50" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1608,15 +1456,12 @@
         <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>1</v>
+        <v>0.9999999999999996</v>
       </c>
       <c r="E51" t="n">
         <v>0</v>
       </c>
       <c r="F51" t="n">
-        <v>0</v>
-      </c>
-      <c r="G51" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1639,9 +1484,6 @@
       <c r="F52" t="n">
         <v>0</v>
       </c>
-      <c r="G52" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -1662,9 +1504,6 @@
       <c r="F53" t="n">
         <v>0</v>
       </c>
-      <c r="G53" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -1685,9 +1524,6 @@
       <c r="F54" t="n">
         <v>0</v>
       </c>
-      <c r="G54" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -1700,15 +1536,12 @@
         <v>0</v>
       </c>
       <c r="D55" t="n">
-        <v>1</v>
+        <v>0.9999999999999996</v>
       </c>
       <c r="E55" t="n">
         <v>0</v>
       </c>
       <c r="F55" t="n">
-        <v>0</v>
-      </c>
-      <c r="G55" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1723,15 +1556,12 @@
         <v>0</v>
       </c>
       <c r="D56" t="n">
-        <v>1</v>
+        <v>0.9999999999999996</v>
       </c>
       <c r="E56" t="n">
         <v>0</v>
       </c>
       <c r="F56" t="n">
-        <v>0</v>
-      </c>
-      <c r="G56" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1754,9 +1584,6 @@
       <c r="F57" t="n">
         <v>0</v>
       </c>
-      <c r="G57" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -1769,15 +1596,12 @@
         <v>0</v>
       </c>
       <c r="D58" t="n">
-        <v>1</v>
+        <v>1.000000000000001</v>
       </c>
       <c r="E58" t="n">
         <v>0</v>
       </c>
       <c r="F58" t="n">
-        <v>0</v>
-      </c>
-      <c r="G58" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1792,15 +1616,12 @@
         <v>0</v>
       </c>
       <c r="D59" t="n">
-        <v>1</v>
+        <v>0.9999999999999993</v>
       </c>
       <c r="E59" t="n">
         <v>0</v>
       </c>
       <c r="F59" t="n">
-        <v>0</v>
-      </c>
-      <c r="G59" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1823,9 +1644,6 @@
       <c r="F60" t="n">
         <v>0</v>
       </c>
-      <c r="G60" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -1846,9 +1664,6 @@
       <c r="F61" t="n">
         <v>0</v>
       </c>
-      <c r="G61" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -1869,9 +1684,6 @@
       <c r="F62" t="n">
         <v>0</v>
       </c>
-      <c r="G62" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -1884,15 +1696,12 @@
         <v>0</v>
       </c>
       <c r="D63" t="n">
-        <v>1</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="E63" t="n">
         <v>0</v>
       </c>
       <c r="F63" t="n">
-        <v>0</v>
-      </c>
-      <c r="G63" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1907,15 +1716,12 @@
         <v>0</v>
       </c>
       <c r="D64" t="n">
-        <v>1</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="E64" t="n">
         <v>0</v>
       </c>
       <c r="F64" t="n">
-        <v>0</v>
-      </c>
-      <c r="G64" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1938,9 +1744,6 @@
       <c r="F65" t="n">
         <v>0</v>
       </c>
-      <c r="G65" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -1961,9 +1764,6 @@
       <c r="F66" t="n">
         <v>0</v>
       </c>
-      <c r="G66" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -1984,9 +1784,6 @@
       <c r="F67" t="n">
         <v>0</v>
       </c>
-      <c r="G67" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -1999,15 +1796,12 @@
         <v>0</v>
       </c>
       <c r="D68" t="n">
-        <v>1</v>
+        <v>0.9999999999999993</v>
       </c>
       <c r="E68" t="n">
         <v>0</v>
       </c>
       <c r="F68" t="n">
-        <v>0</v>
-      </c>
-      <c r="G68" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2030,9 +1824,6 @@
       <c r="F69" t="n">
         <v>0</v>
       </c>
-      <c r="G69" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -2045,15 +1836,12 @@
         <v>0</v>
       </c>
       <c r="D70" t="n">
-        <v>1</v>
+        <v>1.000000000000125</v>
       </c>
       <c r="E70" t="n">
         <v>0</v>
       </c>
       <c r="F70" t="n">
-        <v>0</v>
-      </c>
-      <c r="G70" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2068,15 +1856,12 @@
         <v>0</v>
       </c>
       <c r="D71" t="n">
-        <v>1</v>
+        <v>1.000000000000265</v>
       </c>
       <c r="E71" t="n">
         <v>0</v>
       </c>
       <c r="F71" t="n">
-        <v>0</v>
-      </c>
-      <c r="G71" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2091,15 +1876,12 @@
         <v>0</v>
       </c>
       <c r="D72" t="n">
-        <v>1</v>
+        <v>1.000000000000406</v>
       </c>
       <c r="E72" t="n">
         <v>0</v>
       </c>
       <c r="F72" t="n">
-        <v>0</v>
-      </c>
-      <c r="G72" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2114,15 +1896,12 @@
         <v>0</v>
       </c>
       <c r="D73" t="n">
-        <v>1</v>
+        <v>1.000000000000546</v>
       </c>
       <c r="E73" t="n">
         <v>0</v>
       </c>
       <c r="F73" t="n">
-        <v>0</v>
-      </c>
-      <c r="G73" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2137,15 +1916,12 @@
         <v>0</v>
       </c>
       <c r="D74" t="n">
-        <v>1</v>
+        <v>1.000000000000687</v>
       </c>
       <c r="E74" t="n">
         <v>0</v>
       </c>
       <c r="F74" t="n">
-        <v>0</v>
-      </c>
-      <c r="G74" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2157,18 +1933,15 @@
         <v>573.15</v>
       </c>
       <c r="C75" t="n">
-        <v>0</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="D75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E75" t="n">
         <v>0</v>
       </c>
       <c r="F75" t="n">
-        <v>0</v>
-      </c>
-      <c r="G75" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2180,18 +1953,15 @@
         <v>573.15</v>
       </c>
       <c r="C76" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D76" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E76" t="n">
         <v>0</v>
       </c>
       <c r="F76" t="n">
-        <v>0</v>
-      </c>
-      <c r="G76" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2203,18 +1973,15 @@
         <v>573.15</v>
       </c>
       <c r="C77" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D77" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E77" t="n">
         <v>0</v>
       </c>
       <c r="F77" t="n">
-        <v>0</v>
-      </c>
-      <c r="G77" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2237,9 +2004,6 @@
       <c r="F78" t="n">
         <v>0</v>
       </c>
-      <c r="G78" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -2260,9 +2024,6 @@
       <c r="F79" t="n">
         <v>0</v>
       </c>
-      <c r="G79" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -2283,9 +2044,6 @@
       <c r="F80" t="n">
         <v>0</v>
       </c>
-      <c r="G80" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -2306,9 +2064,6 @@
       <c r="F81" t="n">
         <v>0</v>
       </c>
-      <c r="G81" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
@@ -2318,7 +2073,7 @@
         <v>573.15</v>
       </c>
       <c r="C82" t="n">
-        <v>1</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="D82" t="n">
         <v>0</v>
@@ -2327,9 +2082,6 @@
         <v>0</v>
       </c>
       <c r="F82" t="n">
-        <v>0</v>
-      </c>
-      <c r="G82" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2352,9 +2104,6 @@
       <c r="F83" t="n">
         <v>0</v>
       </c>
-      <c r="G83" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -2375,9 +2124,6 @@
       <c r="F84" t="n">
         <v>0</v>
       </c>
-      <c r="G84" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -2387,7 +2133,7 @@
         <v>573.15</v>
       </c>
       <c r="C85" t="n">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="D85" t="n">
         <v>0</v>
@@ -2396,9 +2142,6 @@
         <v>0</v>
       </c>
       <c r="F85" t="n">
-        <v>0</v>
-      </c>
-      <c r="G85" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2421,9 +2164,6 @@
       <c r="F86" t="n">
         <v>0</v>
       </c>
-      <c r="G86" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -2444,9 +2184,6 @@
       <c r="F87" t="n">
         <v>0</v>
       </c>
-      <c r="G87" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
@@ -2467,9 +2204,6 @@
       <c r="F88" t="n">
         <v>0</v>
       </c>
-      <c r="G88" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -2479,7 +2213,7 @@
         <v>573.15</v>
       </c>
       <c r="C89" t="n">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="D89" t="n">
         <v>0</v>
@@ -2488,9 +2222,6 @@
         <v>0</v>
       </c>
       <c r="F89" t="n">
-        <v>0</v>
-      </c>
-      <c r="G89" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2502,7 +2233,7 @@
         <v>573.15</v>
       </c>
       <c r="C90" t="n">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="D90" t="n">
         <v>0</v>
@@ -2511,9 +2242,6 @@
         <v>0</v>
       </c>
       <c r="F90" t="n">
-        <v>0</v>
-      </c>
-      <c r="G90" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2536,9 +2264,6 @@
       <c r="F91" t="n">
         <v>0</v>
       </c>
-      <c r="G91" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -2559,9 +2284,6 @@
       <c r="F92" t="n">
         <v>0</v>
       </c>
-      <c r="G92" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
@@ -2582,9 +2304,6 @@
       <c r="F93" t="n">
         <v>0</v>
       </c>
-      <c r="G93" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
@@ -2605,9 +2324,6 @@
       <c r="F94" t="n">
         <v>0</v>
       </c>
-      <c r="G94" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
@@ -2628,9 +2344,6 @@
       <c r="F95" t="n">
         <v>0</v>
       </c>
-      <c r="G95" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -2651,9 +2364,6 @@
       <c r="F96" t="n">
         <v>0</v>
       </c>
-      <c r="G96" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
@@ -2674,9 +2384,6 @@
       <c r="F97" t="n">
         <v>0</v>
       </c>
-      <c r="G97" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
@@ -2697,9 +2404,6 @@
       <c r="F98" t="n">
         <v>0</v>
       </c>
-      <c r="G98" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
@@ -2720,9 +2424,6 @@
       <c r="F99" t="n">
         <v>0</v>
       </c>
-      <c r="G99" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
@@ -2743,9 +2444,6 @@
       <c r="F100" t="n">
         <v>0</v>
       </c>
-      <c r="G100" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
@@ -2766,9 +2464,6 @@
       <c r="F101" t="n">
         <v>0</v>
       </c>
-      <c r="G101" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
@@ -2789,9 +2484,6 @@
       <c r="F102" t="n">
         <v>0</v>
       </c>
-      <c r="G102" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
@@ -2812,9 +2504,6 @@
       <c r="F103" t="n">
         <v>0</v>
       </c>
-      <c r="G103" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
@@ -2835,9 +2524,6 @@
       <c r="F104" t="n">
         <v>0</v>
       </c>
-      <c r="G104" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
@@ -2858,9 +2544,6 @@
       <c r="F105" t="n">
         <v>0</v>
       </c>
-      <c r="G105" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
@@ -2881,9 +2564,6 @@
       <c r="F106" t="n">
         <v>0</v>
       </c>
-      <c r="G106" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -2904,9 +2584,6 @@
       <c r="F107" t="n">
         <v>0</v>
       </c>
-      <c r="G107" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -2927,9 +2604,6 @@
       <c r="F108" t="n">
         <v>0</v>
       </c>
-      <c r="G108" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -2950,9 +2624,6 @@
       <c r="F109" t="n">
         <v>0</v>
       </c>
-      <c r="G109" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -2973,9 +2644,6 @@
       <c r="F110" t="n">
         <v>0</v>
       </c>
-      <c r="G110" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -2985,7 +2653,7 @@
         <v>573.15</v>
       </c>
       <c r="C111" t="n">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="D111" t="n">
         <v>0</v>
@@ -2994,9 +2662,6 @@
         <v>0</v>
       </c>
       <c r="F111" t="n">
-        <v>0</v>
-      </c>
-      <c r="G111" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3019,9 +2684,6 @@
       <c r="F112" t="n">
         <v>0</v>
       </c>
-      <c r="G112" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -3042,9 +2704,6 @@
       <c r="F113" t="n">
         <v>0</v>
       </c>
-      <c r="G113" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -3065,9 +2724,6 @@
       <c r="F114" t="n">
         <v>0</v>
       </c>
-      <c r="G114" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -3088,9 +2744,6 @@
       <c r="F115" t="n">
         <v>0</v>
       </c>
-      <c r="G115" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -3111,9 +2764,6 @@
       <c r="F116" t="n">
         <v>0</v>
       </c>
-      <c r="G116" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -3134,9 +2784,6 @@
       <c r="F117" t="n">
         <v>0</v>
       </c>
-      <c r="G117" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -3157,9 +2804,6 @@
       <c r="F118" t="n">
         <v>0</v>
       </c>
-      <c r="G118" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -3169,7 +2813,7 @@
         <v>573.15</v>
       </c>
       <c r="C119" t="n">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="D119" t="n">
         <v>0</v>
@@ -3178,9 +2822,6 @@
         <v>0</v>
       </c>
       <c r="F119" t="n">
-        <v>0</v>
-      </c>
-      <c r="G119" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3203,9 +2844,6 @@
       <c r="F120" t="n">
         <v>0</v>
       </c>
-      <c r="G120" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
@@ -3226,9 +2864,6 @@
       <c r="F121" t="n">
         <v>0</v>
       </c>
-      <c r="G121" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
@@ -3249,9 +2884,6 @@
       <c r="F122" t="n">
         <v>0</v>
       </c>
-      <c r="G122" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
@@ -3272,9 +2904,6 @@
       <c r="F123" t="n">
         <v>0</v>
       </c>
-      <c r="G123" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
@@ -3295,9 +2924,6 @@
       <c r="F124" t="n">
         <v>0</v>
       </c>
-      <c r="G124" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -3307,7 +2933,7 @@
         <v>573.15</v>
       </c>
       <c r="C125" t="n">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="D125" t="n">
         <v>0</v>
@@ -3316,9 +2942,6 @@
         <v>0</v>
       </c>
       <c r="F125" t="n">
-        <v>0</v>
-      </c>
-      <c r="G125" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3341,9 +2964,6 @@
       <c r="F126" t="n">
         <v>0</v>
       </c>
-      <c r="G126" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
@@ -3364,9 +2984,6 @@
       <c r="F127" t="n">
         <v>0</v>
       </c>
-      <c r="G127" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -3387,9 +3004,6 @@
       <c r="F128" t="n">
         <v>0</v>
       </c>
-      <c r="G128" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
@@ -3410,9 +3024,6 @@
       <c r="F129" t="n">
         <v>0</v>
       </c>
-      <c r="G129" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
@@ -3422,7 +3033,7 @@
         <v>573.15</v>
       </c>
       <c r="C130" t="n">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="D130" t="n">
         <v>0</v>
@@ -3431,9 +3042,6 @@
         <v>0</v>
       </c>
       <c r="F130" t="n">
-        <v>0</v>
-      </c>
-      <c r="G130" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3456,9 +3064,6 @@
       <c r="F131" t="n">
         <v>0</v>
       </c>
-      <c r="G131" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
@@ -3479,9 +3084,6 @@
       <c r="F132" t="n">
         <v>0</v>
       </c>
-      <c r="G132" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
@@ -3502,9 +3104,6 @@
       <c r="F133" t="n">
         <v>0</v>
       </c>
-      <c r="G133" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
@@ -3525,9 +3124,6 @@
       <c r="F134" t="n">
         <v>0</v>
       </c>
-      <c r="G134" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -3548,9 +3144,6 @@
       <c r="F135" t="n">
         <v>0</v>
       </c>
-      <c r="G135" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -3571,9 +3164,6 @@
       <c r="F136" t="n">
         <v>0</v>
       </c>
-      <c r="G136" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
@@ -3583,7 +3173,7 @@
         <v>573.15</v>
       </c>
       <c r="C137" t="n">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="D137" t="n">
         <v>0</v>
@@ -3592,9 +3182,6 @@
         <v>0</v>
       </c>
       <c r="F137" t="n">
-        <v>0</v>
-      </c>
-      <c r="G137" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3606,7 +3193,7 @@
         <v>573.15</v>
       </c>
       <c r="C138" t="n">
-        <v>1</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="D138" t="n">
         <v>0</v>
@@ -3615,9 +3202,6 @@
         <v>0</v>
       </c>
       <c r="F138" t="n">
-        <v>0</v>
-      </c>
-      <c r="G138" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3640,9 +3224,6 @@
       <c r="F139" t="n">
         <v>0</v>
       </c>
-      <c r="G139" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -3663,9 +3244,6 @@
       <c r="F140" t="n">
         <v>0</v>
       </c>
-      <c r="G140" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
@@ -3686,9 +3264,6 @@
       <c r="F141" t="n">
         <v>0</v>
       </c>
-      <c r="G141" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -3709,9 +3284,6 @@
       <c r="F142" t="n">
         <v>0</v>
       </c>
-      <c r="G142" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
@@ -3732,9 +3304,6 @@
       <c r="F143" t="n">
         <v>0</v>
       </c>
-      <c r="G143" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -3755,9 +3324,6 @@
       <c r="F144" t="n">
         <v>0</v>
       </c>
-      <c r="G144" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -3778,9 +3344,6 @@
       <c r="F145" t="n">
         <v>0</v>
       </c>
-      <c r="G145" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -3801,9 +3364,6 @@
       <c r="F146" t="n">
         <v>0</v>
       </c>
-      <c r="G146" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -3824,9 +3384,6 @@
       <c r="F147" t="n">
         <v>0</v>
       </c>
-      <c r="G147" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -3847,9 +3404,6 @@
       <c r="F148" t="n">
         <v>0</v>
       </c>
-      <c r="G148" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
@@ -3859,7 +3413,7 @@
         <v>573.15</v>
       </c>
       <c r="C149" t="n">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="D149" t="n">
         <v>0</v>
@@ -3868,9 +3422,6 @@
         <v>0</v>
       </c>
       <c r="F149" t="n">
-        <v>0</v>
-      </c>
-      <c r="G149" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3893,9 +3444,6 @@
       <c r="F150" t="n">
         <v>0</v>
       </c>
-      <c r="G150" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
@@ -3914,9 +3462,6 @@
         <v>0</v>
       </c>
       <c r="F151" t="n">
-        <v>0</v>
-      </c>
-      <c r="G151" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>